<commit_message>
finish create budget test
</commit_message>
<xml_diff>
--- a/src/main/java/resources/CreateBudget_TC.xlsx
+++ b/src/main/java/resources/CreateBudget_TC.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="3255"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16965" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="CreateBudget" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:I24"/>
 </workbook>
 </file>
 
@@ -228,7 +228,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -263,7 +263,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finish sign up test
</commit_message>
<xml_diff>
--- a/src/main/java/resources/CreateBudget_TC.xlsx
+++ b/src/main/java/resources/CreateBudget_TC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="21390" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22305" windowHeight="4725" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CreateBudget" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="BudgetaForm" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K26"/>
+  <oleSize ref="A85:H99"/>
 </workbook>
 </file>
 
@@ -1491,7 +1491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -2116,7 +2116,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A5" sqref="A5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2670,8 +2670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE123"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="X89" sqref="X89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
change the calculation method
</commit_message>
<xml_diff>
--- a/src/main/java/resources/CreateBudget_TC.xlsx
+++ b/src/main/java/resources/CreateBudget_TC.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="321">
   <si>
     <t>id</t>
   </si>
@@ -2738,7 +2738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -3009,23 +3009,23 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>177</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3">
+        <v>10</v>
+      </c>
       <c r="I10" s="3">
-        <v>500</v>
+        <v>22222</v>
       </c>
       <c r="J10" s="3">
         <v>2</v>
@@ -3033,7 +3033,9 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+      <c r="N10" s="3">
+        <v>2</v>
+      </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
         <v>55</v>
@@ -3048,19 +3050,19 @@
         <v>2016</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>210</v>
+        <v>172</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>228</v>
+        <v>176</v>
       </c>
       <c r="X10" s="7" t="s">
-        <v>229</v>
+        <v>175</v>
       </c>
       <c r="Y10" s="7" t="b">
         <v>1</v>
@@ -3072,7 +3074,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>83</v>
@@ -3080,15 +3082,17 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3">
+        <v>20</v>
+      </c>
       <c r="I11" s="3">
-        <v>600</v>
+        <v>25352</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -3100,28 +3104,28 @@
         <v>55</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R11" s="3">
         <v>2015</v>
       </c>
       <c r="S11" s="3">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="V11" s="3" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="X11" s="7" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="Y11" s="7" t="b">
         <v>1</v>
@@ -3131,9 +3135,9 @@
       <c r="AB11" s="12"/>
       <c r="AC11" s="12"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>83</v>
@@ -3144,14 +3148,16 @@
         <v>163</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3">
-        <v>7000</v>
-      </c>
-      <c r="J12" s="3"/>
+        <v>500</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2</v>
+      </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -3170,19 +3176,19 @@
         <v>2016</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="X12" s="7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="Y12" s="7" t="b">
         <v>1</v>
@@ -3194,7 +3200,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>83</v>
@@ -3202,15 +3208,15 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3">
-        <v>8000</v>
+        <v>600</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -3231,19 +3237,19 @@
         <v>2016</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="Y13" s="7" t="b">
         <v>1</v>
@@ -3255,7 +3261,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>83</v>
@@ -3263,17 +3269,15 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="3">
-        <v>10</v>
-      </c>
+      <c r="H14" s="3"/>
       <c r="I14" s="3">
-        <v>1200</v>
+        <v>7000</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -3294,19 +3298,19 @@
         <v>2016</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="V14" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="X14" s="7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="Y14" s="7" t="b">
         <v>1</v>
@@ -3318,7 +3322,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>83</v>
@@ -3329,14 +3333,12 @@
         <v>171</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3">
-        <v>20</v>
-      </c>
+      <c r="H15" s="3"/>
       <c r="I15" s="3">
-        <v>25352</v>
+        <v>8000</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -3357,19 +3359,19 @@
         <v>2016</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="V15" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="X15" s="7" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="Y15" s="7" t="b">
         <v>1</v>
@@ -3381,10 +3383,10 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -3396,14 +3398,12 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I16" s="3">
-        <v>330</v>
-      </c>
-      <c r="J16" s="3">
-        <v>5</v>
-      </c>
+        <v>1200</v>
+      </c>
+      <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -3422,19 +3422,19 @@
         <v>2016</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>194</v>
+        <v>224</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="X16" s="7" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="Y16" s="7" t="b">
         <v>1</v>
@@ -3446,45 +3446,63 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="3">
-        <v>2017</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3">
+        <v>2</v>
+      </c>
       <c r="I17" s="3">
-        <v>200</v>
-      </c>
-      <c r="J17" s="3"/>
+        <v>330</v>
+      </c>
+      <c r="J17" s="3">
+        <v>5</v>
+      </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="R17" s="3">
+        <v>2015</v>
+      </c>
+      <c r="S17" s="3">
         <v>2016</v>
       </c>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3" t="b">
-        <v>0</v>
+      <c r="T17" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="Y17" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
@@ -3493,23 +3511,23 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D18" s="3">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -3517,10 +3535,18 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
+      <c r="P18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="R18" s="3">
+        <v>2015</v>
+      </c>
+      <c r="S18" s="3">
+        <v>2015</v>
+      </c>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
@@ -3536,40 +3562,42 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>155</v>
+        <v>17</v>
       </c>
       <c r="D19" s="3">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3">
-        <v>500</v>
-      </c>
-      <c r="J19" s="3">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3">
-        <v>10</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="3">
-        <v>2</v>
-      </c>
+      <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
+      <c r="P19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R19" s="3">
+        <v>2015</v>
+      </c>
+      <c r="S19" s="3">
+        <v>2018</v>
+      </c>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
@@ -3585,16 +3613,16 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>18</v>
+        <v>155</v>
       </c>
       <c r="D20" s="3">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -3609,10 +3637,10 @@
       <c r="K20" s="3">
         <v>10</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="3"/>
+      <c r="M20" s="3">
         <v>2</v>
       </c>
-      <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3" t="s">
@@ -3625,23 +3653,13 @@
         <v>2015</v>
       </c>
       <c r="S20" s="3">
-        <v>2015</v>
-      </c>
-      <c r="T20" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="U20" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="V20" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="W20" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="X20" s="3" t="s">
-        <v>150</v>
-      </c>
+        <v>2018</v>
+      </c>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
       <c r="Y20" s="3" t="b">
         <v>0</v>
       </c>
@@ -3652,7 +3670,7 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>144</v>
@@ -3692,25 +3710,25 @@
         <v>2015</v>
       </c>
       <c r="S21" s="3">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="V21" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="X21" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Y21" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
@@ -3719,39 +3737,63 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D22" s="3">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3">
-        <v>200</v>
-      </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+        <v>500</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2</v>
+      </c>
+      <c r="K22" s="3">
+        <v>10</v>
+      </c>
+      <c r="L22" s="3">
+        <v>2</v>
+      </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
+      <c r="P22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R22" s="3">
+        <v>2015</v>
+      </c>
+      <c r="S22" s="3">
+        <v>2018</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="Y22" s="3" t="b">
         <v>1</v>
       </c>
@@ -3762,21 +3804,23 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
-        <v>163</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2015</v>
+      </c>
+      <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -3784,10 +3828,18 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
+      <c r="P23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R23" s="3">
+        <v>2015</v>
+      </c>
+      <c r="S23" s="3">
+        <v>2018</v>
+      </c>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
@@ -3803,7 +3855,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>78</v>
@@ -3817,46 +3869,32 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3">
-        <v>2000</v>
-      </c>
-      <c r="J24" s="3">
-        <v>1</v>
-      </c>
+        <v>5000</v>
+      </c>
+      <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="3">
-        <v>1</v>
-      </c>
+      <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R24" s="3">
         <v>2015</v>
       </c>
       <c r="S24" s="3">
-        <v>2016</v>
-      </c>
-      <c r="T24" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="U24" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="V24" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="W24" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="X24" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="Y24" s="7" t="b">
+        <v>2018</v>
+      </c>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3" t="b">
         <v>1</v>
       </c>
       <c r="Z24" s="12"/>
@@ -3866,7 +3904,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>78</v>
@@ -3874,24 +3912,22 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="3">
-        <v>10</v>
-      </c>
+      <c r="H25" s="3"/>
       <c r="I25" s="3">
-        <v>22222</v>
+        <v>2000</v>
       </c>
       <c r="J25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3" t="s">
@@ -3907,19 +3943,19 @@
         <v>2016</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="U25" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="V25" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="X25" s="7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="Y25" s="7" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Update Signup test: Password requirements - password must be at least 8 characters and have at least one number and one letter
</commit_message>
<xml_diff>
--- a/src/main/java/resources/CreateBudget_TC.xlsx
+++ b/src/main/java/resources/CreateBudget_TC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20805" windowHeight="5175" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20805" windowHeight="5175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CreateBudget" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="329">
   <si>
     <t>id</t>
   </si>
@@ -980,6 +980,30 @@
   </si>
   <si>
     <t>Nov</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>abcd1234</t>
+  </si>
+  <si>
+    <t>InvalidPass</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>ahlamTest@gmail.com</t>
+  </si>
+  <si>
+    <t>ahlamTes1t@gmail.com</t>
+  </si>
+  <si>
+    <t>ahlamTest2@gmail.com</t>
+  </si>
+  <si>
+    <t>aaaaaaaa</t>
   </si>
 </sst>
 </file>
@@ -2181,16 +2205,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:J5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="20.625" customWidth="1"/>
+    <col min="7" max="8" width="9.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
@@ -2245,30 +2271,32 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>39</v>
+        <v>325</v>
       </c>
       <c r="F3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1</v>
+      <c r="G3" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>324</v>
       </c>
       <c r="I3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>31</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -2279,28 +2307,28 @@
         <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>326</v>
       </c>
       <c r="F4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3">
-        <v>2</v>
+      <c r="G4" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>328</v>
       </c>
       <c r="I4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>34</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2308,7 +2336,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>44</v>
@@ -2317,101 +2345,198 @@
         <v>44</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>45</v>
+        <v>327</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="3">
-        <v>4</v>
+        <v>123456789</v>
       </c>
       <c r="H5" s="3">
-        <v>5</v>
+        <v>123456789</v>
       </c>
       <c r="I5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>70</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="F6" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="3">
-        <v>3</v>
-      </c>
-      <c r="H6" s="3">
-        <v>3</v>
+      <c r="G6" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>322</v>
       </c>
       <c r="I6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>69</v>
+        <v>41</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="F7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>5</v>
-      </c>
-      <c r="H7" s="3">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>322</v>
       </c>
       <c r="I7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="J7" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
+      <c r="H8" s="3">
+        <v>5</v>
+      </c>
+      <c r="I8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="I9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5</v>
+      </c>
+      <c r="I10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F8" s="3"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="E7" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId1"/>
+    <hyperlink ref="E8" r:id="rId2"/>
+    <hyperlink ref="E9" r:id="rId3"/>
+    <hyperlink ref="E10" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId5"/>
+    <hyperlink ref="E4" r:id="rId6"/>
+    <hyperlink ref="E5" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2738,8 +2863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix failed test from the last Jenkins run: Scenarios, Sign up and Account settings
</commit_message>
<xml_diff>
--- a/src/main/java/resources/CreateBudget_TC.xlsx
+++ b/src/main/java/resources/CreateBudget_TC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="20196" windowHeight="8664" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22110" windowHeight="5475" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CreateBudget" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="BudgetaForm" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E18"/>
+  <oleSize ref="A1:Q17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="327">
   <si>
     <t>id</t>
   </si>
@@ -996,6 +996,9 @@
   </si>
   <si>
     <t>aaaaaaaa</t>
+  </si>
+  <si>
+    <t>a1234567</t>
   </si>
 </sst>
 </file>
@@ -1588,21 +1591,21 @@
       <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.59765625" customWidth="1"/>
-    <col min="10" max="10" width="17.09765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.09765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.09765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.625" customWidth="1"/>
+    <col min="10" max="10" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1625,7 +1628,7 @@
       <c r="O1" s="24"/>
       <c r="P1" s="24"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1675,7 +1678,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1722,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1766,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1816,7 +1819,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1863,7 +1866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1910,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2004,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2051,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2145,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2208,18 +2211,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.59765625" customWidth="1"/>
-    <col min="7" max="8" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.69921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.625" customWidth="1"/>
+    <col min="7" max="8" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2507,11 +2510,11 @@
       <c r="F10" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="3">
-        <v>5</v>
-      </c>
-      <c r="H10" s="3">
-        <v>5</v>
+      <c r="G10" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>326</v>
       </c>
       <c r="I10" s="3" t="b">
         <v>0</v>
@@ -2549,14 +2552,14 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2864,40 +2867,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="28.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.5" customWidth="1"/>
-    <col min="14" max="14" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.59765625" customWidth="1"/>
-    <col min="16" max="16" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.09765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.69921875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="19.59765625" customWidth="1"/>
-    <col min="24" max="24" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.69921875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.625" customWidth="1"/>
+    <col min="16" max="16" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="19.625" customWidth="1"/>
+    <col min="24" max="24" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>146</v>
       </c>
@@ -2912,7 +2915,7 @@
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2947,7 +2950,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2982,7 +2985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -3017,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>145</v>
       </c>
@@ -3050,7 +3053,7 @@
       <c r="AB8" s="13"/>
       <c r="AC8" s="13"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -3133,7 +3136,7 @@
       <c r="AD9" s="12"/>
       <c r="AE9" s="12"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3198,7 +3201,7 @@
       <c r="AB10" s="12"/>
       <c r="AC10" s="12"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>21</v>
       </c>
@@ -3324,7 +3327,7 @@
       <c r="AB12" s="12"/>
       <c r="AC12" s="12"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>17</v>
       </c>
@@ -3385,7 +3388,7 @@
       <c r="AB13" s="12"/>
       <c r="AC13" s="12"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>18</v>
       </c>
@@ -3446,7 +3449,7 @@
       <c r="AB14" s="12"/>
       <c r="AC14" s="12"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>19</v>
       </c>
@@ -3507,7 +3510,7 @@
       <c r="AB15" s="12"/>
       <c r="AC15" s="12"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>20</v>
       </c>
@@ -3570,7 +3573,7 @@
       <c r="AB16" s="12"/>
       <c r="AC16" s="12"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -3635,7 +3638,7 @@
       <c r="AB17" s="12"/>
       <c r="AC17" s="12"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -3686,7 +3689,7 @@
       <c r="AB18" s="12"/>
       <c r="AC18" s="12"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2</v>
       </c>
@@ -3737,7 +3740,7 @@
       <c r="AB19" s="12"/>
       <c r="AC19" s="12"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>3</v>
       </c>
@@ -3794,7 +3797,7 @@
       <c r="AB20" s="12"/>
       <c r="AC20" s="12"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>4</v>
       </c>
@@ -3861,7 +3864,7 @@
       <c r="AB21" s="12"/>
       <c r="AC21" s="12"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>5</v>
       </c>
@@ -3928,7 +3931,7 @@
       <c r="AB22" s="12"/>
       <c r="AC22" s="12"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>6</v>
       </c>
@@ -3979,7 +3982,7 @@
       <c r="AB23" s="12"/>
       <c r="AC23" s="12"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>7</v>
       </c>
@@ -4028,7 +4031,7 @@
       <c r="AB24" s="12"/>
       <c r="AC24" s="12"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>8</v>
       </c>
@@ -4091,7 +4094,7 @@
       <c r="AB25" s="12"/>
       <c r="AC25" s="12"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>10</v>
       </c>
@@ -4152,7 +4155,7 @@
       <c r="AB26" s="12"/>
       <c r="AC26" s="12"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>11</v>
       </c>
@@ -4213,7 +4216,7 @@
       <c r="AB27" s="12"/>
       <c r="AC27" s="12"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>12</v>
       </c>
@@ -4274,7 +4277,7 @@
       <c r="AB28" s="12"/>
       <c r="AC28" s="12"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>13</v>
       </c>
@@ -4337,7 +4340,7 @@
       <c r="AB29" s="12"/>
       <c r="AC29" s="12"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>15</v>
       </c>
@@ -4400,7 +4403,7 @@
       <c r="AB30" s="12"/>
       <c r="AC30" s="12"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -4431,7 +4434,7 @@
       <c r="AB37" s="12"/>
       <c r="AC37" s="12"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A40" s="33" t="s">
         <v>105</v>
       </c>
@@ -4452,7 +4455,7 @@
       <c r="P40" s="15"/>
       <c r="Q40" s="16"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>0</v>
       </c>
@@ -4496,7 +4499,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>1</v>
       </c>
@@ -4540,7 +4543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>2</v>
       </c>
@@ -4584,7 +4587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>112</v>
       </c>
@@ -4612,7 +4615,7 @@
       <c r="W48" s="15"/>
       <c r="X48" s="15"/>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:38" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>0</v>
       </c>
@@ -4672,7 +4675,7 @@
       </c>
       <c r="T49" s="17"/>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:38" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>1</v>
       </c>
@@ -4731,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>2</v>
       </c>
@@ -4790,7 +4793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>3</v>
       </c>
@@ -4849,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>4</v>
       </c>
@@ -4908,7 +4911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
@@ -4929,7 +4932,7 @@
       <c r="R54" s="12"/>
       <c r="S54" s="12"/>
     </row>
-    <row r="55" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
@@ -4950,7 +4953,7 @@
       <c r="R55" s="12"/>
       <c r="S55" s="12"/>
     </row>
-    <row r="56" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
@@ -4971,8 +4974,8 @@
       <c r="R56" s="12"/>
       <c r="S56" s="12"/>
     </row>
-    <row r="57" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
         <v>138</v>
       </c>
@@ -5005,7 +5008,7 @@
       <c r="AB58" s="15"/>
       <c r="AC58" s="15"/>
     </row>
-    <row r="59" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>0</v>
       </c>
@@ -5079,7 +5082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>1</v>
       </c>
@@ -5153,7 +5156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>2</v>
       </c>
@@ -5217,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>3</v>
       </c>
@@ -5281,7 +5284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>4</v>
       </c>
@@ -5355,9 +5358,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="22" t="s">
         <v>136</v>
       </c>
@@ -5384,7 +5387,7 @@
       <c r="V67" s="16"/>
       <c r="W67" s="16"/>
     </row>
-    <row r="68" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>0</v>
       </c>
@@ -5446,7 +5449,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>1</v>
       </c>
@@ -5494,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>2</v>
       </c>
@@ -5554,9 +5557,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
         <v>137</v>
       </c>
@@ -5586,7 +5589,7 @@
       <c r="Y77" s="21"/>
       <c r="Z77" s="21"/>
     </row>
-    <row r="78" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>0</v>
       </c>
@@ -5666,7 +5669,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>1</v>
       </c>
@@ -5704,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>2</v>
       </c>
@@ -5742,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>3</v>
       </c>
@@ -5780,7 +5783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>4</v>
       </c>
@@ -5818,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>5</v>
       </c>
@@ -5870,7 +5873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>6</v>
       </c>
@@ -5942,7 +5945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>7</v>
       </c>
@@ -6008,7 +6011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>8</v>
       </c>
@@ -6054,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>9</v>
       </c>
@@ -6092,7 +6095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>10</v>
       </c>
@@ -6130,7 +6133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>11</v>
       </c>
@@ -6200,7 +6203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>12</v>
       </c>
@@ -6246,7 +6249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>13</v>
       </c>
@@ -6308,7 +6311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>14</v>
       </c>
@@ -6376,7 +6379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>15</v>
       </c>
@@ -6446,7 +6449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>16</v>
       </c>
@@ -6516,7 +6519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>17</v>
       </c>
@@ -6578,7 +6581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>18</v>
       </c>
@@ -6626,7 +6629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>19</v>
       </c>
@@ -6688,7 +6691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>20</v>
       </c>
@@ -6756,7 +6759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>21</v>
       </c>
@@ -6826,7 +6829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>22</v>
       </c>
@@ -6894,7 +6897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>23</v>
       </c>
@@ -6958,7 +6961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -6986,7 +6989,7 @@
       <c r="Y102" s="3"/>
       <c r="Z102" s="3"/>
     </row>
-    <row r="103" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
@@ -7011,8 +7014,8 @@
       <c r="V103" s="12"/>
       <c r="W103" s="12"/>
     </row>
-    <row r="104" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A105" s="28" t="s">
         <v>139</v>
       </c>
@@ -7028,7 +7031,7 @@
       <c r="K105" s="28"/>
       <c r="L105" s="28"/>
     </row>
-    <row r="106" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>0</v>
       </c>
@@ -7066,7 +7069,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>1</v>
       </c>
@@ -7104,7 +7107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>2</v>
       </c>
@@ -7142,11 +7145,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A113" s="28" t="s">
         <v>300</v>
       </c>
@@ -7164,7 +7167,7 @@
       <c r="M113" s="28"/>
       <c r="N113" s="28"/>
     </row>
-    <row r="114" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
         <v>0</v>
       </c>
@@ -7208,7 +7211,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>1</v>
       </c>
@@ -7248,7 +7251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>2</v>
       </c>
@@ -7288,9 +7291,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A120" s="28" t="s">
         <v>311</v>
       </c>
@@ -7308,7 +7311,7 @@
       <c r="M120" s="28"/>
       <c r="N120" s="28"/>
     </row>
-    <row r="121" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A121" s="18" t="s">
         <v>0</v>
       </c>
@@ -7352,7 +7355,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="122" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>1</v>
       </c>
@@ -7392,7 +7395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>2</v>
       </c>
@@ -7432,7 +7435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="B124" s="12"/>
       <c r="C124" s="12"/>
@@ -7448,7 +7451,7 @@
       <c r="M124" s="12"/>
       <c r="N124" s="14"/>
     </row>
-    <row r="125" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="B125" s="12"/>
       <c r="C125" s="12"/>
@@ -7464,7 +7467,7 @@
       <c r="M125" s="12"/>
       <c r="N125" s="14"/>
     </row>
-    <row r="126" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A126" s="28" t="s">
         <v>312</v>
       </c>
@@ -7482,7 +7485,7 @@
       <c r="M126" s="28"/>
       <c r="N126" s="28"/>
     </row>
-    <row r="127" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A127" s="18" t="s">
         <v>0</v>
       </c>
@@ -7526,7 +7529,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="128" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>1</v>
       </c>
@@ -7566,7 +7569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>2</v>
       </c>
@@ -7606,7 +7609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="B130" s="12"/>
       <c r="C130" s="12"/>
@@ -7622,7 +7625,7 @@
       <c r="M130" s="12"/>
       <c r="N130" s="14"/>
     </row>
-    <row r="131" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="B131" s="12"/>
       <c r="C131" s="12"/>
@@ -7638,7 +7641,7 @@
       <c r="M131" s="12"/>
       <c r="N131" s="14"/>
     </row>
-    <row r="132" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="B132" s="12"/>
       <c r="C132" s="12"/>
@@ -7654,7 +7657,7 @@
       <c r="M132" s="12"/>
       <c r="N132" s="14"/>
     </row>
-    <row r="133" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="B133" s="12"/>
       <c r="C133" s="12"/>
@@ -7670,7 +7673,7 @@
       <c r="M133" s="12"/>
       <c r="N133" s="14"/>
     </row>
-    <row r="134" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="B134" s="12"/>
       <c r="C134" s="12"/>
@@ -7686,7 +7689,7 @@
       <c r="M134" s="12"/>
       <c r="N134" s="14"/>
     </row>
-    <row r="135" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A135" s="20" t="s">
         <v>302</v>
       </c>
@@ -7710,7 +7713,7 @@
       <c r="S135" s="20"/>
       <c r="T135" s="20"/>
     </row>
-    <row r="136" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>0</v>
       </c>
@@ -7772,7 +7775,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="137" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>1</v>
       </c>
@@ -7830,7 +7833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>2</v>
       </c>
@@ -7886,7 +7889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="B139" s="12"/>
       <c r="C139" s="12"/>
@@ -7902,7 +7905,7 @@
       <c r="M139" s="12"/>
       <c r="N139" s="14"/>
     </row>
-    <row r="140" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="B140" s="12"/>
       <c r="C140" s="12"/>
@@ -7918,7 +7921,7 @@
       <c r="M140" s="12"/>
       <c r="N140" s="14"/>
     </row>
-    <row r="141" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
@@ -7934,7 +7937,7 @@
       <c r="M141" s="12"/>
       <c r="N141" s="14"/>
     </row>
-    <row r="142" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A142" s="20" t="s">
         <v>313</v>
       </c>
@@ -7959,7 +7962,7 @@
       <c r="T142" s="20"/>
       <c r="U142" s="20"/>
     </row>
-    <row r="143" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>0</v>
       </c>
@@ -8024,7 +8027,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="144" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>1</v>
       </c>
@@ -8064,7 +8067,7 @@
       </c>
       <c r="V144" s="3"/>
     </row>
-    <row r="145" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>2</v>
       </c>
@@ -8100,7 +8103,7 @@
       </c>
       <c r="V145" s="3"/>
     </row>
-    <row r="146" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>3</v>
       </c>
@@ -8138,7 +8141,7 @@
       </c>
       <c r="V146" s="3"/>
     </row>
-    <row r="147" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>4</v>
       </c>
@@ -8194,7 +8197,7 @@
       </c>
       <c r="V147" s="3"/>
     </row>
-    <row r="148" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>5</v>
       </c>
@@ -8250,7 +8253,7 @@
       </c>
       <c r="V148" s="3"/>
     </row>
-    <row r="149" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>6</v>
       </c>
@@ -8286,7 +8289,7 @@
       </c>
       <c r="V149" s="3"/>
     </row>
-    <row r="150" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>7</v>
       </c>
@@ -8320,7 +8323,7 @@
       </c>
       <c r="V150" s="3"/>
     </row>
-    <row r="151" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>8</v>
       </c>
@@ -8374,7 +8377,7 @@
       </c>
       <c r="V151" s="3"/>
     </row>
-    <row r="152" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>9</v>
       </c>
@@ -8430,7 +8433,7 @@
       </c>
       <c r="V152" s="3"/>
     </row>
-    <row r="153" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>10</v>
       </c>
@@ -8484,7 +8487,7 @@
       </c>
       <c r="V153" s="3"/>
     </row>
-    <row r="154" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>11</v>
       </c>
@@ -8538,7 +8541,7 @@
       </c>
       <c r="V154" s="3"/>
     </row>
-    <row r="155" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>12</v>
       </c>
@@ -8592,7 +8595,7 @@
       </c>
       <c r="V155" s="3"/>
     </row>
-    <row r="156" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>13</v>
       </c>
@@ -8648,7 +8651,7 @@
       </c>
       <c r="V156" s="3"/>
     </row>
-    <row r="157" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>14</v>
       </c>
@@ -8706,7 +8709,7 @@
       </c>
       <c r="V157" s="3"/>
     </row>
-    <row r="158" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>15</v>
       </c>
@@ -8762,7 +8765,7 @@
       </c>
       <c r="V158" s="3"/>
     </row>
-    <row r="159" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>16</v>
       </c>
@@ -8818,7 +8821,7 @@
       </c>
       <c r="V159" s="3"/>
     </row>
-    <row r="160" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>17</v>
       </c>
@@ -8872,7 +8875,7 @@
       </c>
       <c r="V160" s="3"/>
     </row>
-    <row r="161" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>18</v>
       </c>
@@ -8926,7 +8929,7 @@
       </c>
       <c r="V161" s="3"/>
     </row>
-    <row r="162" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>19</v>
       </c>
@@ -8980,7 +8983,7 @@
       </c>
       <c r="V162" s="3"/>
     </row>
-    <row r="163" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>20</v>
       </c>
@@ -9036,7 +9039,7 @@
       </c>
       <c r="V163" s="3"/>
     </row>
-    <row r="164" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>21</v>
       </c>
@@ -9092,7 +9095,7 @@
       </c>
       <c r="V164" s="3"/>
     </row>
-    <row r="165" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -9116,7 +9119,7 @@
       <c r="U165" s="3"/>
       <c r="V165" s="3"/>
     </row>
-    <row r="166" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -9140,7 +9143,7 @@
       <c r="U166" s="3"/>
       <c r="V166" s="3"/>
     </row>
-    <row r="167" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
@@ -9164,7 +9167,7 @@
       <c r="U167" s="3"/>
       <c r="V167" s="3"/>
     </row>
-    <row r="168" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="B168" s="12"/>
       <c r="C168" s="12"/>
@@ -9186,7 +9189,7 @@
       <c r="S168" s="12"/>
       <c r="T168" s="14"/>
     </row>
-    <row r="169" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="B169" s="12"/>
       <c r="C169" s="12"/>
@@ -9208,7 +9211,7 @@
       <c r="S169" s="12"/>
       <c r="T169" s="14"/>
     </row>
-    <row r="170" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="B170" s="12"/>
       <c r="C170" s="12"/>
@@ -9230,7 +9233,7 @@
       <c r="S170" s="12"/>
       <c r="T170" s="14"/>
     </row>
-    <row r="171" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="B171" s="12"/>
       <c r="C171" s="12"/>
@@ -9252,7 +9255,7 @@
       <c r="S171" s="12"/>
       <c r="T171" s="14"/>
     </row>
-    <row r="172" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="B172" s="12"/>
       <c r="C172" s="12"/>
@@ -9274,7 +9277,7 @@
       <c r="S172" s="12"/>
       <c r="T172" s="14"/>
     </row>
-    <row r="173" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="B173" s="12"/>
       <c r="C173" s="12"/>
@@ -9296,7 +9299,7 @@
       <c r="S173" s="12"/>
       <c r="T173" s="14"/>
     </row>
-    <row r="174" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="B174" s="12"/>
       <c r="C174" s="12"/>
@@ -9318,7 +9321,7 @@
       <c r="S174" s="12"/>
       <c r="T174" s="14"/>
     </row>
-    <row r="175" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A175" s="20" t="s">
         <v>316</v>
       </c>
@@ -9343,7 +9346,7 @@
       <c r="T175" s="20"/>
       <c r="U175" s="20"/>
     </row>
-    <row r="176" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>0</v>
       </c>
@@ -9408,7 +9411,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="177" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>1</v>
       </c>
@@ -9447,7 +9450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>2</v>
       </c>
@@ -9482,7 +9485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>3</v>
       </c>
@@ -9519,7 +9522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>4</v>
       </c>
@@ -9574,7 +9577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>5</v>
       </c>
@@ -9629,7 +9632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>6</v>
       </c>
@@ -9664,7 +9667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>7</v>
       </c>
@@ -9697,7 +9700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>8</v>
       </c>
@@ -9750,7 +9753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>9</v>
       </c>
@@ -9805,7 +9808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>10</v>
       </c>
@@ -9858,7 +9861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>11</v>
       </c>
@@ -9911,7 +9914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>12</v>
       </c>
@@ -9964,7 +9967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>13</v>
       </c>
@@ -10019,7 +10022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>14</v>
       </c>
@@ -10076,7 +10079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>15</v>
       </c>
@@ -10131,7 +10134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>16</v>
       </c>
@@ -10186,7 +10189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>17</v>
       </c>
@@ -10239,7 +10242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>18</v>
       </c>
@@ -10292,7 +10295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>19</v>
       </c>
@@ -10345,7 +10348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>20</v>
       </c>
@@ -10400,7 +10403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>21</v>
       </c>
@@ -10455,7 +10458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
@@ -10478,7 +10481,7 @@
       <c r="T198" s="3"/>
       <c r="U198" s="3"/>
     </row>
-    <row r="199" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A199" s="3"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
@@ -10501,7 +10504,7 @@
       <c r="T199" s="3"/>
       <c r="U199" s="3"/>
     </row>
-    <row r="200" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A200" s="3"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
@@ -10524,7 +10527,7 @@
       <c r="T200" s="3"/>
       <c r="U200" s="3"/>
     </row>
-    <row r="201" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" s="12"/>
       <c r="C201" s="12"/>
@@ -10540,10 +10543,10 @@
       <c r="M201" s="12"/>
       <c r="N201" s="14"/>
     </row>
-    <row r="202" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
     <row r="204" spans="1:38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A205" s="28" t="s">
         <v>140</v>
       </c>
@@ -10559,7 +10562,7 @@
       <c r="K205" s="28"/>
       <c r="L205" s="28"/>
     </row>
-    <row r="206" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A206" s="10" t="s">
         <v>0</v>
       </c>
@@ -10597,7 +10600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="207" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>1</v>
       </c>
@@ -10635,7 +10638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>2</v>
       </c>
@@ -10673,9 +10676,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="212" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="213" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A213" s="28" t="s">
         <v>141</v>
       </c>
@@ -10691,7 +10694,7 @@
       <c r="K213" s="28"/>
       <c r="L213" s="28"/>
     </row>
-    <row r="214" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A214" s="10" t="s">
         <v>0</v>
       </c>
@@ -10729,7 +10732,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="215" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>1</v>
       </c>
@@ -10767,7 +10770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>2</v>
       </c>
@@ -10805,9 +10808,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="220" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="221" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A221" s="28" t="s">
         <v>314</v>
       </c>
@@ -10825,7 +10828,7 @@
       <c r="M221" s="28"/>
       <c r="N221" s="28"/>
     </row>
-    <row r="222" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A222" s="18" t="s">
         <v>0</v>
       </c>
@@ -10869,7 +10872,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="223" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>1</v>
       </c>
@@ -10909,7 +10912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>2</v>
       </c>
@@ -10949,9 +10952,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="234" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="235" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A235" s="21" t="s">
         <v>315</v>
       </c>
@@ -10981,7 +10984,7 @@
       <c r="Y235" s="21"/>
       <c r="Z235" s="21"/>
     </row>
-    <row r="236" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
         <v>0</v>
       </c>
@@ -11061,7 +11064,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="237" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
         <v>18</v>
       </c>
@@ -11117,7 +11120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
         <v>19</v>
       </c>
@@ -11179,7 +11182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A239" s="3">
         <v>20</v>
       </c>
@@ -11247,7 +11250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A240" s="3">
         <v>21</v>
       </c>
@@ -11317,7 +11320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A241" s="3">
         <v>22</v>
       </c>
@@ -11385,7 +11388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A242" s="3">
         <v>23</v>
       </c>
@@ -11449,7 +11452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A243" s="3">
         <v>12</v>
       </c>
@@ -11565,7 +11568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A245" s="3">
         <v>14</v>
       </c>
@@ -11633,7 +11636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A246" s="3">
         <v>15</v>
       </c>
@@ -11703,7 +11706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A247" s="3">
         <v>16</v>
       </c>
@@ -11773,7 +11776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A248" s="3">
         <v>17</v>
       </c>
@@ -11835,7 +11838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A249" s="3">
         <v>1</v>
       </c>
@@ -11873,7 +11876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A250" s="3">
         <v>2</v>
       </c>
@@ -11911,7 +11914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A251" s="3">
         <v>3</v>
       </c>
@@ -11949,7 +11952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A252" s="3">
         <v>4</v>
       </c>
@@ -11987,7 +11990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A253" s="3">
         <v>5</v>
       </c>
@@ -12039,7 +12042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A254" s="3">
         <v>6</v>
       </c>
@@ -12111,7 +12114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A255" s="3">
         <v>7</v>
       </c>
@@ -12223,7 +12226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A257" s="3">
         <v>9</v>
       </c>
@@ -12269,7 +12272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A258" s="3">
         <v>10</v>
       </c>
@@ -12307,7 +12310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A259" s="3">
         <v>11</v>
       </c>
@@ -12377,22 +12380,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="261" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="262" spans="1:38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="260" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="261" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
+    <row r="262" spans="1:38" customFormat="1" ht="13.9" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A221:N221"/>
-    <mergeCell ref="A120:N120"/>
-    <mergeCell ref="A126:N126"/>
-    <mergeCell ref="A213:L213"/>
-    <mergeCell ref="A205:L205"/>
     <mergeCell ref="A113:N113"/>
     <mergeCell ref="A105:L105"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A8:Y8"/>
     <mergeCell ref="A40:N40"/>
     <mergeCell ref="A48:S48"/>
+    <mergeCell ref="A221:N221"/>
+    <mergeCell ref="A120:N120"/>
+    <mergeCell ref="A126:N126"/>
+    <mergeCell ref="A213:L213"/>
+    <mergeCell ref="A205:L205"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change in excel file CreateBudget_TC
</commit_message>
<xml_diff>
--- a/src/main/java/resources/CreateBudget_TC.xlsx
+++ b/src/main/java/resources/CreateBudget_TC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22110" windowHeight="5475" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22110" windowHeight="5055" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CreateBudget" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="BudgetaForm" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -1260,6 +1261,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1267,9 +1271,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2863,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2897,19 +2898,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3017,33 +3018,33 @@
       </c>
     </row>
     <row r="8" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="31"/>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="31"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28"/>
       <c r="Z8" s="13"/>
       <c r="AA8" s="13"/>
       <c r="AB8" s="13"/>
@@ -3227,7 +3228,7 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11" s="12"/>
       <c r="AA11" s="12"/>
@@ -3537,7 +3538,7 @@
       <c r="AB16" s="12"/>
       <c r="AC16" s="12"/>
     </row>
-    <row r="17" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>8</v>
       </c>
@@ -5484,34 +5485,34 @@
       </c>
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A76" s="31" t="s">
+      <c r="A76" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="B76" s="31"/>
-      <c r="C76" s="31"/>
-      <c r="D76" s="31"/>
-      <c r="E76" s="31"/>
-      <c r="F76" s="31"/>
-      <c r="G76" s="31"/>
-      <c r="H76" s="31"/>
-      <c r="I76" s="31"/>
-      <c r="J76" s="31"/>
-      <c r="K76" s="31"/>
-      <c r="L76" s="31"/>
-      <c r="M76" s="31"/>
-      <c r="N76" s="31"/>
-      <c r="O76" s="31"/>
-      <c r="P76" s="31"/>
-      <c r="Q76" s="31"/>
-      <c r="R76" s="31"/>
-      <c r="S76" s="31"/>
-      <c r="T76" s="31"/>
-      <c r="U76" s="31"/>
-      <c r="V76" s="31"/>
-      <c r="W76" s="31"/>
-      <c r="X76" s="31"/>
-      <c r="Y76" s="31"/>
-      <c r="Z76" s="31"/>
+      <c r="B76" s="28"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="28"/>
+      <c r="F76" s="28"/>
+      <c r="G76" s="28"/>
+      <c r="H76" s="28"/>
+      <c r="I76" s="28"/>
+      <c r="J76" s="28"/>
+      <c r="K76" s="28"/>
+      <c r="L76" s="28"/>
+      <c r="M76" s="28"/>
+      <c r="N76" s="28"/>
+      <c r="O76" s="28"/>
+      <c r="P76" s="28"/>
+      <c r="Q76" s="28"/>
+      <c r="R76" s="28"/>
+      <c r="S76" s="28"/>
+      <c r="T76" s="28"/>
+      <c r="U76" s="28"/>
+      <c r="V76" s="28"/>
+      <c r="W76" s="28"/>
+      <c r="X76" s="28"/>
+      <c r="Y76" s="28"/>
+      <c r="Z76" s="28"/>
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
@@ -7855,29 +7856,29 @@
       <c r="N140" s="14"/>
     </row>
     <row r="141" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A141" s="31" t="s">
+      <c r="A141" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="B141" s="31"/>
-      <c r="C141" s="31"/>
-      <c r="D141" s="31"/>
-      <c r="E141" s="31"/>
-      <c r="F141" s="31"/>
-      <c r="G141" s="31"/>
-      <c r="H141" s="31"/>
-      <c r="I141" s="31"/>
-      <c r="J141" s="31"/>
-      <c r="K141" s="31"/>
-      <c r="L141" s="31"/>
-      <c r="M141" s="31"/>
-      <c r="N141" s="31"/>
-      <c r="O141" s="31"/>
-      <c r="P141" s="31"/>
-      <c r="Q141" s="31"/>
-      <c r="R141" s="31"/>
-      <c r="S141" s="31"/>
-      <c r="T141" s="31"/>
-      <c r="U141" s="31"/>
+      <c r="B141" s="28"/>
+      <c r="C141" s="28"/>
+      <c r="D141" s="28"/>
+      <c r="E141" s="28"/>
+      <c r="F141" s="28"/>
+      <c r="G141" s="28"/>
+      <c r="H141" s="28"/>
+      <c r="I141" s="28"/>
+      <c r="J141" s="28"/>
+      <c r="K141" s="28"/>
+      <c r="L141" s="28"/>
+      <c r="M141" s="28"/>
+      <c r="N141" s="28"/>
+      <c r="O141" s="28"/>
+      <c r="P141" s="28"/>
+      <c r="Q141" s="28"/>
+      <c r="R141" s="28"/>
+      <c r="S141" s="28"/>
+      <c r="T141" s="28"/>
+      <c r="U141" s="28"/>
     </row>
     <row r="142" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
@@ -9239,29 +9240,29 @@
       <c r="T173" s="14"/>
     </row>
     <row r="174" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A174" s="31" t="s">
+      <c r="A174" s="28" t="s">
         <v>316</v>
       </c>
-      <c r="B174" s="31"/>
-      <c r="C174" s="31"/>
-      <c r="D174" s="31"/>
-      <c r="E174" s="31"/>
-      <c r="F174" s="31"/>
-      <c r="G174" s="31"/>
-      <c r="H174" s="31"/>
-      <c r="I174" s="31"/>
-      <c r="J174" s="31"/>
-      <c r="K174" s="31"/>
-      <c r="L174" s="31"/>
-      <c r="M174" s="31"/>
-      <c r="N174" s="31"/>
-      <c r="O174" s="31"/>
-      <c r="P174" s="31"/>
-      <c r="Q174" s="31"/>
-      <c r="R174" s="31"/>
-      <c r="S174" s="31"/>
-      <c r="T174" s="31"/>
-      <c r="U174" s="31"/>
+      <c r="B174" s="28"/>
+      <c r="C174" s="28"/>
+      <c r="D174" s="28"/>
+      <c r="E174" s="28"/>
+      <c r="F174" s="28"/>
+      <c r="G174" s="28"/>
+      <c r="H174" s="28"/>
+      <c r="I174" s="28"/>
+      <c r="J174" s="28"/>
+      <c r="K174" s="28"/>
+      <c r="L174" s="28"/>
+      <c r="M174" s="28"/>
+      <c r="N174" s="28"/>
+      <c r="O174" s="28"/>
+      <c r="P174" s="28"/>
+      <c r="Q174" s="28"/>
+      <c r="R174" s="28"/>
+      <c r="S174" s="28"/>
+      <c r="T174" s="28"/>
+      <c r="U174" s="28"/>
     </row>
     <row r="175" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
@@ -10864,34 +10865,34 @@
       </c>
     </row>
     <row r="234" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A234" s="31" t="s">
+      <c r="A234" s="28" t="s">
         <v>315</v>
       </c>
-      <c r="B234" s="31"/>
-      <c r="C234" s="31"/>
-      <c r="D234" s="31"/>
-      <c r="E234" s="31"/>
-      <c r="F234" s="31"/>
-      <c r="G234" s="31"/>
-      <c r="H234" s="31"/>
-      <c r="I234" s="31"/>
-      <c r="J234" s="31"/>
-      <c r="K234" s="31"/>
-      <c r="L234" s="31"/>
-      <c r="M234" s="31"/>
-      <c r="N234" s="31"/>
-      <c r="O234" s="31"/>
-      <c r="P234" s="31"/>
-      <c r="Q234" s="31"/>
-      <c r="R234" s="31"/>
-      <c r="S234" s="31"/>
-      <c r="T234" s="31"/>
-      <c r="U234" s="31"/>
-      <c r="V234" s="31"/>
-      <c r="W234" s="31"/>
-      <c r="X234" s="31"/>
-      <c r="Y234" s="31"/>
-      <c r="Z234" s="31"/>
+      <c r="B234" s="28"/>
+      <c r="C234" s="28"/>
+      <c r="D234" s="28"/>
+      <c r="E234" s="28"/>
+      <c r="F234" s="28"/>
+      <c r="G234" s="28"/>
+      <c r="H234" s="28"/>
+      <c r="I234" s="28"/>
+      <c r="J234" s="28"/>
+      <c r="K234" s="28"/>
+      <c r="L234" s="28"/>
+      <c r="M234" s="28"/>
+      <c r="N234" s="28"/>
+      <c r="O234" s="28"/>
+      <c r="P234" s="28"/>
+      <c r="Q234" s="28"/>
+      <c r="R234" s="28"/>
+      <c r="S234" s="28"/>
+      <c r="T234" s="28"/>
+      <c r="U234" s="28"/>
+      <c r="V234" s="28"/>
+      <c r="W234" s="28"/>
+      <c r="X234" s="28"/>
+      <c r="Y234" s="28"/>
+      <c r="Z234" s="28"/>
     </row>
     <row r="235" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A235" s="4" t="s">
@@ -12307,6 +12308,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A112:N112"/>
+    <mergeCell ref="A104:L104"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:Y8"/>
+    <mergeCell ref="A39:N39"/>
+    <mergeCell ref="A47:S47"/>
+    <mergeCell ref="A76:Z76"/>
     <mergeCell ref="A234:Z234"/>
     <mergeCell ref="A220:N220"/>
     <mergeCell ref="A119:N119"/>
@@ -12315,13 +12323,6 @@
     <mergeCell ref="A204:L204"/>
     <mergeCell ref="A174:U174"/>
     <mergeCell ref="A141:U141"/>
-    <mergeCell ref="A112:N112"/>
-    <mergeCell ref="A104:L104"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:Y8"/>
-    <mergeCell ref="A39:N39"/>
-    <mergeCell ref="A47:S47"/>
-    <mergeCell ref="A76:Z76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix failed tests --> Scenario, vesrsio , budget settings
</commit_message>
<xml_diff>
--- a/src/main/java/resources/CreateBudget_TC.xlsx
+++ b/src/main/java/resources/CreateBudget_TC.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="322">
   <si>
     <t>id</t>
   </si>
@@ -1245,6 +1245,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1252,9 +1255,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2755,10 +2755,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE252"/>
+  <dimension ref="A1:AE251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I33" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="C250" sqref="C250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2791,19 +2791,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2876,33 +2876,33 @@
       </c>
     </row>
     <row r="7" spans="1:31" ht="13.9" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="31"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
       <c r="Z7" s="13"/>
       <c r="AA7" s="13"/>
       <c r="AB7" s="13"/>
@@ -5248,34 +5248,34 @@
       </c>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A73" s="31" t="s">
+      <c r="A73" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="B73" s="31"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="31"/>
-      <c r="E73" s="31"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="31"/>
-      <c r="I73" s="31"/>
-      <c r="J73" s="31"/>
-      <c r="K73" s="31"/>
-      <c r="L73" s="31"/>
-      <c r="M73" s="31"/>
-      <c r="N73" s="31"/>
-      <c r="O73" s="31"/>
-      <c r="P73" s="31"/>
-      <c r="Q73" s="31"/>
-      <c r="R73" s="31"/>
-      <c r="S73" s="31"/>
-      <c r="T73" s="31"/>
-      <c r="U73" s="31"/>
-      <c r="V73" s="31"/>
-      <c r="W73" s="31"/>
-      <c r="X73" s="31"/>
-      <c r="Y73" s="31"/>
-      <c r="Z73" s="31"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="28"/>
+      <c r="H73" s="28"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="28"/>
+      <c r="K73" s="28"/>
+      <c r="L73" s="28"/>
+      <c r="M73" s="28"/>
+      <c r="N73" s="28"/>
+      <c r="O73" s="28"/>
+      <c r="P73" s="28"/>
+      <c r="Q73" s="28"/>
+      <c r="R73" s="28"/>
+      <c r="S73" s="28"/>
+      <c r="T73" s="28"/>
+      <c r="U73" s="28"/>
+      <c r="V73" s="28"/>
+      <c r="W73" s="28"/>
+      <c r="X73" s="28"/>
+      <c r="Y73" s="28"/>
+      <c r="Z73" s="28"/>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
@@ -7619,29 +7619,29 @@
       <c r="N137" s="14"/>
     </row>
     <row r="138" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A138" s="31" t="s">
+      <c r="A138" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="B138" s="31"/>
-      <c r="C138" s="31"/>
-      <c r="D138" s="31"/>
-      <c r="E138" s="31"/>
-      <c r="F138" s="31"/>
-      <c r="G138" s="31"/>
-      <c r="H138" s="31"/>
-      <c r="I138" s="31"/>
-      <c r="J138" s="31"/>
-      <c r="K138" s="31"/>
-      <c r="L138" s="31"/>
-      <c r="M138" s="31"/>
-      <c r="N138" s="31"/>
-      <c r="O138" s="31"/>
-      <c r="P138" s="31"/>
-      <c r="Q138" s="31"/>
-      <c r="R138" s="31"/>
-      <c r="S138" s="31"/>
-      <c r="T138" s="31"/>
-      <c r="U138" s="31"/>
+      <c r="B138" s="28"/>
+      <c r="C138" s="28"/>
+      <c r="D138" s="28"/>
+      <c r="E138" s="28"/>
+      <c r="F138" s="28"/>
+      <c r="G138" s="28"/>
+      <c r="H138" s="28"/>
+      <c r="I138" s="28"/>
+      <c r="J138" s="28"/>
+      <c r="K138" s="28"/>
+      <c r="L138" s="28"/>
+      <c r="M138" s="28"/>
+      <c r="N138" s="28"/>
+      <c r="O138" s="28"/>
+      <c r="P138" s="28"/>
+      <c r="Q138" s="28"/>
+      <c r="R138" s="28"/>
+      <c r="S138" s="28"/>
+      <c r="T138" s="28"/>
+      <c r="U138" s="28"/>
     </row>
     <row r="139" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
@@ -9003,29 +9003,29 @@
       <c r="T170" s="14"/>
     </row>
     <row r="171" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A171" s="31" t="s">
+      <c r="A171" s="28" t="s">
         <v>311</v>
       </c>
-      <c r="B171" s="31"/>
-      <c r="C171" s="31"/>
-      <c r="D171" s="31"/>
-      <c r="E171" s="31"/>
-      <c r="F171" s="31"/>
-      <c r="G171" s="31"/>
-      <c r="H171" s="31"/>
-      <c r="I171" s="31"/>
-      <c r="J171" s="31"/>
-      <c r="K171" s="31"/>
-      <c r="L171" s="31"/>
-      <c r="M171" s="31"/>
-      <c r="N171" s="31"/>
-      <c r="O171" s="31"/>
-      <c r="P171" s="31"/>
-      <c r="Q171" s="31"/>
-      <c r="R171" s="31"/>
-      <c r="S171" s="31"/>
-      <c r="T171" s="31"/>
-      <c r="U171" s="31"/>
+      <c r="B171" s="28"/>
+      <c r="C171" s="28"/>
+      <c r="D171" s="28"/>
+      <c r="E171" s="28"/>
+      <c r="F171" s="28"/>
+      <c r="G171" s="28"/>
+      <c r="H171" s="28"/>
+      <c r="I171" s="28"/>
+      <c r="J171" s="28"/>
+      <c r="K171" s="28"/>
+      <c r="L171" s="28"/>
+      <c r="M171" s="28"/>
+      <c r="N171" s="28"/>
+      <c r="O171" s="28"/>
+      <c r="P171" s="28"/>
+      <c r="Q171" s="28"/>
+      <c r="R171" s="28"/>
+      <c r="S171" s="28"/>
+      <c r="T171" s="28"/>
+      <c r="U171" s="28"/>
     </row>
     <row r="172" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
@@ -10588,34 +10588,34 @@
       </c>
     </row>
     <row r="230" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A230" s="31" t="s">
+      <c r="A230" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="B230" s="31"/>
-      <c r="C230" s="31"/>
-      <c r="D230" s="31"/>
-      <c r="E230" s="31"/>
-      <c r="F230" s="31"/>
-      <c r="G230" s="31"/>
-      <c r="H230" s="31"/>
-      <c r="I230" s="31"/>
-      <c r="J230" s="31"/>
-      <c r="K230" s="31"/>
-      <c r="L230" s="31"/>
-      <c r="M230" s="31"/>
-      <c r="N230" s="31"/>
-      <c r="O230" s="31"/>
-      <c r="P230" s="31"/>
-      <c r="Q230" s="31"/>
-      <c r="R230" s="31"/>
-      <c r="S230" s="31"/>
-      <c r="T230" s="31"/>
-      <c r="U230" s="31"/>
-      <c r="V230" s="31"/>
-      <c r="W230" s="31"/>
-      <c r="X230" s="31"/>
-      <c r="Y230" s="31"/>
-      <c r="Z230" s="31"/>
+      <c r="B230" s="28"/>
+      <c r="C230" s="28"/>
+      <c r="D230" s="28"/>
+      <c r="E230" s="28"/>
+      <c r="F230" s="28"/>
+      <c r="G230" s="28"/>
+      <c r="H230" s="28"/>
+      <c r="I230" s="28"/>
+      <c r="J230" s="28"/>
+      <c r="K230" s="28"/>
+      <c r="L230" s="28"/>
+      <c r="M230" s="28"/>
+      <c r="N230" s="28"/>
+      <c r="O230" s="28"/>
+      <c r="P230" s="28"/>
+      <c r="Q230" s="28"/>
+      <c r="R230" s="28"/>
+      <c r="S230" s="28"/>
+      <c r="T230" s="28"/>
+      <c r="U230" s="28"/>
+      <c r="V230" s="28"/>
+      <c r="W230" s="28"/>
+      <c r="X230" s="28"/>
+      <c r="Y230" s="28"/>
+      <c r="Z230" s="28"/>
     </row>
     <row r="231" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A231" s="4" t="s">
@@ -11777,7 +11777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A250" s="3">
         <v>19</v>
       </c>
@@ -11801,13 +11801,13 @@
         <v>14</v>
       </c>
       <c r="M250" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N250" s="3">
         <v>2015</v>
       </c>
       <c r="O250" s="3">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="P250" s="3"/>
       <c r="Q250" s="3"/>
@@ -11820,7 +11820,7 @@
       <c r="X250" s="3"/>
       <c r="Y250" s="3"/>
       <c r="Z250" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:26" x14ac:dyDescent="0.2">
@@ -11833,18 +11833,22 @@
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
       <c r="E251" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="F251" s="3"/>
       <c r="G251" s="3"/>
-      <c r="H251" s="3"/>
+      <c r="H251" s="3">
+        <v>5</v>
+      </c>
       <c r="I251" s="3">
-        <v>2000</v>
-      </c>
-      <c r="J251" s="3"/>
+        <v>300</v>
+      </c>
+      <c r="J251" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="K251" s="3"/>
       <c r="L251" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M251" s="3" t="s">
         <v>15</v>
@@ -11855,92 +11859,50 @@
       <c r="O251" s="3">
         <v>2015</v>
       </c>
-      <c r="P251" s="3"/>
-      <c r="Q251" s="3"/>
-      <c r="R251" s="3"/>
-      <c r="S251" s="3"/>
-      <c r="T251" s="3"/>
-      <c r="U251" s="3"/>
-      <c r="V251" s="3"/>
-      <c r="W251" s="3"/>
-      <c r="X251" s="3"/>
-      <c r="Y251" s="3"/>
+      <c r="P251" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q251" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="R251" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="S251" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="T251" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="U251" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V251" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="W251" s="3">
+        <v>2015</v>
+      </c>
+      <c r="X251" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y251" s="3" t="s">
+        <v>241</v>
+      </c>
       <c r="Z251" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A252" s="3">
-        <v>21</v>
-      </c>
-      <c r="B252" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C252" s="3"/>
-      <c r="D252" s="3"/>
-      <c r="E252" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F252" s="3"/>
-      <c r="G252" s="3"/>
-      <c r="H252" s="3">
-        <v>5</v>
-      </c>
-      <c r="I252" s="3">
-        <v>300</v>
-      </c>
-      <c r="J252" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K252" s="3"/>
-      <c r="L252" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M252" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N252" s="3">
-        <v>2015</v>
-      </c>
-      <c r="O252" s="3">
-        <v>2015</v>
-      </c>
-      <c r="P252" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q252" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="R252" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="S252" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="T252" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="U252" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="V252" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="W252" s="3">
-        <v>2015</v>
-      </c>
-      <c r="X252" s="3">
-        <v>2</v>
-      </c>
-      <c r="Y252" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="Z252" s="3" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A109:N109"/>
+    <mergeCell ref="A101:L101"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A7:Y7"/>
+    <mergeCell ref="A37:N37"/>
+    <mergeCell ref="A44:S44"/>
+    <mergeCell ref="A73:Z73"/>
+    <mergeCell ref="A54:X54"/>
     <mergeCell ref="A230:Z230"/>
     <mergeCell ref="A217:N217"/>
     <mergeCell ref="A116:N116"/>
@@ -11949,14 +11911,6 @@
     <mergeCell ref="A201:L201"/>
     <mergeCell ref="A171:U171"/>
     <mergeCell ref="A138:U138"/>
-    <mergeCell ref="A109:N109"/>
-    <mergeCell ref="A101:L101"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A7:Y7"/>
-    <mergeCell ref="A37:N37"/>
-    <mergeCell ref="A44:S44"/>
-    <mergeCell ref="A73:Z73"/>
-    <mergeCell ref="A54:X54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>